<commit_message>
updated code a little bit with a data dictionary and default input
</commit_message>
<xml_diff>
--- a/TonganZhao/PaulShinn/Janus/7 and 11pt.xlsx
+++ b/TonganZhao/PaulShinn/Janus/7 and 11pt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2022SpringCodingCamp\TonganZhao\PaulShinn\Janus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E68D4F-51D9-491C-91F6-C415A24F8FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A278ED45-BEED-4D8A-8E4A-DC53AEF11A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="225" windowWidth="23820" windowHeight="14175" activeTab="1" xr2:uid="{C112BFFF-7BBC-4FD0-B0CB-837E18384276}"/>
+    <workbookView xWindow="-28440" yWindow="75" windowWidth="18435" windowHeight="14880" activeTab="1" xr2:uid="{C112BFFF-7BBC-4FD0-B0CB-837E18384276}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5579,7 +5579,7 @@
   <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>